<commit_message>
Modified the step 1 instructions
</commit_message>
<xml_diff>
--- a/docs/unit1/5_gantt_charts/(Starter-Workbook)-Class-Gantt-Chart.xlsx
+++ b/docs/unit1/5_gantt_charts/(Starter-Workbook)-Class-Gantt-Chart.xlsx
@@ -5,23 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bw383\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\5_gantt_charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB2F713-A3F8-4A5C-BF43-0F22E706114D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A764EC-5507-4ABE-9F1E-8451B6F80ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="display_week">Sheet1!$C$4</definedName>
-    <definedName name="project_start">Sheet1!$C$3</definedName>
-    <definedName name="task_end" localSheetId="0">Sheet1!$D1</definedName>
-    <definedName name="task_progress" localSheetId="0">Sheet1!$B1</definedName>
-    <definedName name="task_start" localSheetId="0">Sheet1!$C1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -73,7 +66,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    <numFmt numFmtId="167" formatCode="m\-d\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="m\-d\-yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -168,19 +161,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -194,140 +187,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -544,7 +404,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
General cleanup of Gantt chart in-class. Also fixed HW.
</commit_message>
<xml_diff>
--- a/docs/unit1/5_gantt_charts/(Starter-Workbook)-Class-Gantt-Chart.xlsx
+++ b/docs/unit1/5_gantt_charts/(Starter-Workbook)-Class-Gantt-Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\5_gantt_charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/content/docs/unit1/5_gantt_charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A764EC-5507-4ABE-9F1E-8451B6F80ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2811D58-D94A-F841-8692-8C94ECF93C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5780" yWindow="3560" windowWidth="39260" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Company Name</t>
   </si>
@@ -58,15 +55,17 @@
   </si>
   <si>
     <t>Project Lead</t>
+  </si>
+  <si>
+    <t>ASSIGNED TO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    <numFmt numFmtId="165" formatCode="m\-d\-yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m\-d\-yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -79,23 +78,27 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,51 +138,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -401,121 +398,137 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.5703125" style="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>